<commit_message>
Phase2 API - Temperature data capturing from openweathermap
Phase2 added new file for capturing temperature value from
openweathermap

Signed-off-by: Nirupam Ghosh <nirupamghosh.blr@gmail.com>
</commit_message>
<xml_diff>
--- a/testData/data.xlsx
+++ b/testData/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="9">
   <si>
     <t>City</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>23.11</t>
+  </si>
+  <si>
+    <t>21.58</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -539,6 +542,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,7 +557,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E9775D-70EA-4464-99DC-705CD131D218}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -734,6 +745,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Phase3-  Temperature Value comparison between ndtv and oneweathermap
Compariosn of temperature data between ndtv and oneweathermap, if
difference is above 3 result is Fail

Signed-off-by: Nirupam Ghosh <nirupamghosh.blr@gmail.com>
</commit_message>
<xml_diff>
--- a/testData/data.xlsx
+++ b/testData/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirup\eclipse-workspace_2020\ProjectW\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Selenium\Weather-Reporting-Comparator\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CED1FA0-6B79-4A67-B5EF-F1840656CE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701B5741-B83C-436D-BB09-4F4A8334A302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="72" windowWidth="13224" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NDTV" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="6">
   <si>
-    <t>City</t>
+    <t>City_Name</t>
   </si>
   <si>
-    <t>Min</t>
+    <t xml:space="preserve">Temperature in Celsius </t>
   </si>
   <si>
     <t>NDTV_Bengaluru</t>
@@ -43,16 +43,7 @@
     <t>API_Bengaluru</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23.11</t>
-  </si>
-  <si>
-    <t>21.58</t>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -371,15 +362,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -390,7 +382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -398,7 +390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -406,7 +398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -414,7 +406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -422,7 +414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -430,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -438,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -446,107 +438,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -557,16 +453,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E9775D-70EA-4464-99DC-705CD131D218}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -577,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -585,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -593,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -601,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -609,7 +505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -617,7 +513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -625,7 +521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -633,124 +529,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>